<commit_message>
running ucerf scenarios, added examples of ucerf and user-defind ruptures, added wells caprocks examples
</commit_message>
<xml_diff>
--- a/param_dist/wells_caprocks.xlsx
+++ b/param_dist/wells_caprocks.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://slategeotech-my.sharepoint.com/personal/bzheng_slategeotech_com/Documents/CEC/OpenSRA/param_dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{2987D35D-B7D5-480E-B7BB-5CC225CF1AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7B15137-7B82-458F-B865-1D53AF81DD66}"/>
+  <xr:revisionPtr revIDLastSave="264" documentId="8_{2987D35D-B7D5-480E-B7BB-5CC225CF1AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8485C03D-28A7-46B5-85EF-CAE0555B8841}"/>
   <bookViews>
-    <workbookView xWindow="-27480" yWindow="-120" windowWidth="27600" windowHeight="16440" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
+    <workbookView xWindow="-25710" yWindow="-1700" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="level1" sheetId="6" r:id="rId1"/>
     <sheet name="level2" sheetId="5" r:id="rId2"/>
     <sheet name="level3" sheetId="1" r:id="rId3"/>
     <sheet name="fixed" sheetId="7" r:id="rId4"/>
+    <sheet name="fixed_superseded" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="55">
   <si>
     <t>normal</t>
   </si>
@@ -130,9 +131,6 @@
     <t>unitless</t>
   </si>
   <si>
-    <t>user provided</t>
-  </si>
-  <si>
     <t>phi_soil</t>
   </si>
   <si>
@@ -145,9 +143,6 @@
     <t>well mode: 1, 2, 4</t>
   </si>
   <si>
-    <t>h_wh</t>
-  </si>
-  <si>
     <t>mpl_wh</t>
   </si>
   <si>
@@ -167,6 +162,48 @@
   </si>
   <si>
     <t>cemented casing/tubing (True/False)</t>
+  </si>
+  <si>
+    <t>height_wh</t>
+  </si>
+  <si>
+    <t>depends</t>
+  </si>
+  <si>
+    <t>fault depth</t>
+  </si>
+  <si>
+    <t>d_production_casing</t>
+  </si>
+  <si>
+    <t>d_tubing</t>
+  </si>
+  <si>
+    <t>casing_flow</t>
+  </si>
+  <si>
+    <t>outer diameter of production casing</t>
+  </si>
+  <si>
+    <t>outer diameter of tubing</t>
+  </si>
+  <si>
+    <t>flag for whether well is configured for casing flow</t>
+  </si>
+  <si>
+    <t>z_top_of_cement</t>
+  </si>
+  <si>
+    <t>d_production_boring</t>
+  </si>
+  <si>
+    <t>depth to top of cement</t>
+  </si>
+  <si>
+    <t>diameter of production boring</t>
+  </si>
+  <si>
+    <t>z_crossing</t>
   </si>
 </sst>
 </file>
@@ -518,28 +555,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52ECD9D-96F6-4DA0-914B-F81C4D5742D5}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" customWidth="1"/>
+    <col min="9" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -574,7 +610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -590,20 +626,23 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2">
-        <v>45</v>
+      <c r="F2" t="s">
+        <v>42</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>70</v>
       </c>
       <c r="K2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -625,11 +664,17 @@
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="I3">
+        <v>5.1335551817941469E-4</v>
+      </c>
+      <c r="J3">
+        <v>0.20710239733195912</v>
+      </c>
       <c r="K3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -651,86 +696,95 @@
       <c r="G4">
         <v>0.5</v>
       </c>
+      <c r="I4">
+        <v>0.21660284272461347</v>
+      </c>
+      <c r="J4">
+        <v>4.3505843952126355</v>
+      </c>
       <c r="K4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5">
+        <v>457.2</v>
+      </c>
+      <c r="I5">
+        <v>76.2</v>
+      </c>
+      <c r="J5">
+        <v>2362.1999999999998</v>
+      </c>
+      <c r="K5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F5">
-        <v>11.147968000000001</v>
-      </c>
-      <c r="G5">
-        <v>2.5350000000000001</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6">
+        <v>3.9</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>25</v>
-      </c>
-      <c r="H6">
-        <v>20</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7">
-        <v>60</v>
       </c>
       <c r="H7">
         <v>20</v>
@@ -742,72 +796,136 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="B8" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <f>10*0.3048</f>
+        <v>3.048</v>
+      </c>
+      <c r="G9">
+        <f>1*0.3048</f>
+        <v>0.30480000000000002</v>
+      </c>
+      <c r="I9">
+        <f>7*0.3048</f>
+        <v>2.1335999999999999</v>
+      </c>
+      <c r="J9">
+        <f>13*0.3048</f>
+        <v>3.9624000000000001</v>
+      </c>
+      <c r="K9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="F10">
+        <f>60 * 17.87</f>
+        <v>1072.2</v>
+      </c>
+      <c r="G10">
+        <f>10 * 17.87</f>
+        <v>178.70000000000002</v>
+      </c>
+      <c r="I10">
+        <f>20*17.87</f>
+        <v>357.40000000000003</v>
+      </c>
+      <c r="J10">
+        <f>100*17.87</f>
+        <v>1787</v>
+      </c>
+      <c r="K10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="K8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>35</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>29</v>
+      </c>
+      <c r="J11">
         <v>40</v>
       </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="K11" t="s">
         <v>0</v>
       </c>
     </row>
@@ -818,28 +936,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8004289-A966-4581-8188-6DAA3855ADE3}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:K1048576"/>
+      <selection sqref="A1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" customWidth="1"/>
+    <col min="9" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -874,7 +991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -890,20 +1007,23 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2">
-        <v>45</v>
+      <c r="F2" t="s">
+        <v>42</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>70</v>
       </c>
       <c r="K2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -925,11 +1045,17 @@
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="I3">
+        <v>5.1335551817941469E-4</v>
+      </c>
+      <c r="J3">
+        <v>0.20710239733195912</v>
+      </c>
       <c r="K3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -951,86 +1077,95 @@
       <c r="G4">
         <v>0.5</v>
       </c>
+      <c r="I4">
+        <v>0.21660284272461347</v>
+      </c>
+      <c r="J4">
+        <v>4.3505843952126355</v>
+      </c>
       <c r="K4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5">
+        <v>457.2</v>
+      </c>
+      <c r="I5">
+        <v>76.2</v>
+      </c>
+      <c r="J5">
+        <v>2362.1999999999998</v>
+      </c>
+      <c r="K5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F5">
-        <v>11.147968000000001</v>
-      </c>
-      <c r="G5">
-        <v>2.5350000000000001</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6">
+        <v>3.9</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>25</v>
-      </c>
-      <c r="H6">
-        <v>20</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7">
-        <v>60</v>
       </c>
       <c r="H7">
         <v>20</v>
@@ -1042,72 +1177,136 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="B8" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <f>10*0.3048</f>
+        <v>3.048</v>
+      </c>
+      <c r="G9">
+        <f>1*0.3048</f>
+        <v>0.30480000000000002</v>
+      </c>
+      <c r="I9">
+        <f>7*0.3048</f>
+        <v>2.1335999999999999</v>
+      </c>
+      <c r="J9">
+        <f>13*0.3048</f>
+        <v>3.9624000000000001</v>
+      </c>
+      <c r="K9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="F10">
+        <f>60 * 17.87</f>
+        <v>1072.2</v>
+      </c>
+      <c r="G10">
+        <f>10 * 17.87</f>
+        <v>178.70000000000002</v>
+      </c>
+      <c r="I10">
+        <f>20*17.87</f>
+        <v>357.40000000000003</v>
+      </c>
+      <c r="J10">
+        <f>100*17.87</f>
+        <v>1787</v>
+      </c>
+      <c r="K10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="K8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>35</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>29</v>
+      </c>
+      <c r="J11">
         <v>40</v>
       </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="K11" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1118,28 +1317,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38878A27-4F03-488B-A8C6-4048A6415AE1}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:K1048576"/>
+      <selection sqref="A1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" customWidth="1"/>
+    <col min="9" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1174,7 +1372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1190,20 +1388,23 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2">
-        <v>45</v>
+      <c r="F2" t="s">
+        <v>42</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>70</v>
       </c>
       <c r="K2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1225,11 +1426,17 @@
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="I3">
+        <v>5.1335551817941469E-4</v>
+      </c>
+      <c r="J3">
+        <v>0.20710239733195912</v>
+      </c>
       <c r="K3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1251,86 +1458,95 @@
       <c r="G4">
         <v>0.5</v>
       </c>
+      <c r="I4">
+        <v>0.21660284272461347</v>
+      </c>
+      <c r="J4">
+        <v>4.3505843952126355</v>
+      </c>
       <c r="K4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5">
+        <v>457.2</v>
+      </c>
+      <c r="I5">
+        <v>76.2</v>
+      </c>
+      <c r="J5">
+        <v>2362.1999999999998</v>
+      </c>
+      <c r="K5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F5">
-        <v>11.147968000000001</v>
-      </c>
-      <c r="G5">
-        <v>2.5350000000000001</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6">
+        <v>3.9</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>25</v>
-      </c>
-      <c r="H6">
-        <v>20</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7">
-        <v>60</v>
       </c>
       <c r="H7">
         <v>20</v>
@@ -1342,72 +1558,136 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="B8" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <f>10*0.3048</f>
+        <v>3.048</v>
+      </c>
+      <c r="G9">
+        <f>1*0.3048</f>
+        <v>0.30480000000000002</v>
+      </c>
+      <c r="I9">
+        <f>7*0.3048</f>
+        <v>2.1335999999999999</v>
+      </c>
+      <c r="J9">
+        <f>13*0.3048</f>
+        <v>3.9624000000000001</v>
+      </c>
+      <c r="K9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="F10">
+        <f>60 * 17.87</f>
+        <v>1072.2</v>
+      </c>
+      <c r="G10">
+        <f>10 * 17.87</f>
+        <v>178.70000000000002</v>
+      </c>
+      <c r="I10">
+        <f>20*17.87</f>
+        <v>357.40000000000003</v>
+      </c>
+      <c r="J10">
+        <f>100*17.87</f>
+        <v>1787</v>
+      </c>
+      <c r="K10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="K8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>35</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>29</v>
+      </c>
+      <c r="J11">
         <v>40</v>
       </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="K11" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1418,23 +1698,149 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655B523C-3764-4F21-ABAD-95043A0AB93D}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1426202-DCB6-4AB0-8FBC-EA68A4D46263}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1451,29 +1857,29 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -1482,7 +1888,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
made sure code works with above ground and wells caprocks examples, and added an extra example for above ground that uses filters for IM
</commit_message>
<xml_diff>
--- a/param_dist/wells_caprocks.xlsx
+++ b/param_dist/wells_caprocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://slategeotech-my.sharepoint.com/personal/bzheng_slategeotech_com/Documents/CEC/OpenSRA/param_dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="264" documentId="8_{2987D35D-B7D5-480E-B7BB-5CC225CF1AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8485C03D-28A7-46B5-85EF-CAE0555B8841}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="8_{2987D35D-B7D5-480E-B7BB-5CC225CF1AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2080E0E3-5841-4F02-81BF-566B5EB3FE13}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-1700" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
+    <workbookView xWindow="6060" yWindow="1290" windowWidth="23295" windowHeight="14025" activeTab="2" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="level1" sheetId="6" r:id="rId1"/>
@@ -239,8 +239,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,7 +559,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:L1048576"/>
+      <selection sqref="A1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +572,7 @@
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.85546875" customWidth="1"/>
-    <col min="9" max="10" width="7.28515625" customWidth="1"/>
+    <col min="9" max="10" width="10.28515625" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -632,11 +633,11 @@
       <c r="G2">
         <v>10</v>
       </c>
-      <c r="I2">
-        <v>20</v>
+      <c r="I2" s="1">
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="K2" t="s">
         <v>0</v>
@@ -665,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>5.1335551817941469E-4</v>
+        <v>5.1335551817941502E-4</v>
       </c>
       <c r="J3">
         <v>0.20710239733195912</v>
@@ -728,11 +729,8 @@
       <c r="G5">
         <v>457.2</v>
       </c>
-      <c r="I5">
-        <v>76.2</v>
-      </c>
-      <c r="J5">
-        <v>2362.1999999999998</v>
+      <c r="I5" s="1">
+        <v>0</v>
       </c>
       <c r="K5" t="s">
         <v>0</v>
@@ -939,7 +937,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:L1048576"/>
+      <selection sqref="A1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +950,7 @@
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.85546875" customWidth="1"/>
-    <col min="9" max="10" width="7.28515625" customWidth="1"/>
+    <col min="9" max="10" width="10.28515625" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1013,11 +1011,11 @@
       <c r="G2">
         <v>10</v>
       </c>
-      <c r="I2">
-        <v>20</v>
+      <c r="I2" s="1">
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="K2" t="s">
         <v>0</v>
@@ -1046,7 +1044,7 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>5.1335551817941469E-4</v>
+        <v>5.1335551817941502E-4</v>
       </c>
       <c r="J3">
         <v>0.20710239733195912</v>
@@ -1109,11 +1107,8 @@
       <c r="G5">
         <v>457.2</v>
       </c>
-      <c r="I5">
-        <v>76.2</v>
-      </c>
-      <c r="J5">
-        <v>2362.1999999999998</v>
+      <c r="I5" s="1">
+        <v>0</v>
       </c>
       <c r="K5" t="s">
         <v>0</v>
@@ -1319,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38878A27-4F03-488B-A8C6-4048A6415AE1}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:L1048576"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1328,7 @@
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.85546875" customWidth="1"/>
-    <col min="9" max="10" width="7.28515625" customWidth="1"/>
+    <col min="9" max="10" width="10.28515625" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1394,11 +1389,11 @@
       <c r="G2">
         <v>10</v>
       </c>
-      <c r="I2">
-        <v>20</v>
+      <c r="I2" s="1">
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="K2" t="s">
         <v>0</v>
@@ -1427,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>5.1335551817941469E-4</v>
+        <v>5.1335551817941502E-4</v>
       </c>
       <c r="J3">
         <v>0.20710239733195912</v>
@@ -1490,11 +1485,8 @@
       <c r="G5">
         <v>457.2</v>
       </c>
-      <c r="I5">
-        <v>76.2</v>
-      </c>
-      <c r="J5">
-        <v>2362.1999999999998</v>
+      <c r="I5" s="1">
+        <v>0</v>
       </c>
       <c r="K5" t="s">
         <v>0</v>
@@ -1700,8 +1692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655B523C-3764-4F21-ABAD-95043A0AB93D}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated file structure under examples, updated pathing in setupconfig, reorganized CPT params for setupconfig
</commit_message>
<xml_diff>
--- a/param_dist/wells_caprocks.xlsx
+++ b/param_dist/wells_caprocks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barry\OneDrive - SlateGeotech\CEC\OpenSRA\param_dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://slategeotech-my.sharepoint.com/personal/bzheng_slategeotech_com/Documents/CEC/OpenSRA/param_dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBD7CC0-92A3-4F17-810E-D9FA54BC2D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{CDBD7CC0-92A3-4F17-810E-D9FA54BC2D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{833019CE-213E-4B48-B7CE-19E366D47396}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
+    <workbookView xWindow="2550" yWindow="6555" windowWidth="23190" windowHeight="14025" activeTab="1" xr2:uid="{0CF1B192-5A29-435B-821A-1A8E6C927DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="level1" sheetId="6" r:id="rId1"/>
@@ -77,27 +77,15 @@
     <t>theta</t>
   </si>
   <si>
-    <t>fault angle</t>
-  </si>
-  <si>
     <t>w_fc</t>
   </si>
   <si>
-    <t>fault core width</t>
-  </si>
-  <si>
     <t>w_dz</t>
   </si>
   <si>
-    <t>damage zone width</t>
-  </si>
-  <si>
     <t>e_rock</t>
   </si>
   <si>
-    <t>Young's modulus of rock</t>
-  </si>
-  <si>
     <t>GPa</t>
   </si>
   <si>
@@ -107,12 +95,6 @@
     <t>phi_cmt</t>
   </si>
   <si>
-    <t>internal friction angle of cement</t>
-  </si>
-  <si>
-    <t>uniaxial compressive strength of cement</t>
-  </si>
-  <si>
     <t>MPa</t>
   </si>
   <si>
@@ -146,18 +128,9 @@
     <t>mpl_wh</t>
   </si>
   <si>
-    <t>wellhead height, for all modes</t>
-  </si>
-  <si>
-    <t>wellhead mass per length, for all modes</t>
-  </si>
-  <si>
     <t>kg/m</t>
   </si>
   <si>
-    <t>soil friction angle, modes 1 and 2 only</t>
-  </si>
-  <si>
     <t>cement_flag</t>
   </si>
   <si>
@@ -170,9 +143,6 @@
     <t>depends</t>
   </si>
   <si>
-    <t>fault depth</t>
-  </si>
-  <si>
     <t>d_production_casing</t>
   </si>
   <si>
@@ -182,12 +152,6 @@
     <t>casing_flow</t>
   </si>
   <si>
-    <t>outer diameter of production casing</t>
-  </si>
-  <si>
-    <t>outer diameter of tubing</t>
-  </si>
-  <si>
     <t>flag for whether well is configured for casing flow</t>
   </si>
   <si>
@@ -197,13 +161,49 @@
     <t>d_production_boring</t>
   </si>
   <si>
-    <t>depth to top of cement</t>
-  </si>
-  <si>
-    <t>diameter of production boring</t>
-  </si>
-  <si>
     <t>z_crossing</t>
+  </si>
+  <si>
+    <t>[deg] fault angle</t>
+  </si>
+  <si>
+    <t>[m] fault core width</t>
+  </si>
+  <si>
+    <t>[m] damage zone width</t>
+  </si>
+  <si>
+    <t>[m] fault depth</t>
+  </si>
+  <si>
+    <t>[GPa] Young's modulus of rock</t>
+  </si>
+  <si>
+    <t>[deg] internal friction angle of cement</t>
+  </si>
+  <si>
+    <t>[MPa] uniaxial compressive strength of cement</t>
+  </si>
+  <si>
+    <t>[m] wellhead height, for all modes</t>
+  </si>
+  <si>
+    <t>[kg/m] wellhead mass per length, for all modes</t>
+  </si>
+  <si>
+    <t>[deg] soil friction angle, modes 1 and 2 only</t>
+  </si>
+  <si>
+    <t>[m] diameter of production boring</t>
+  </si>
+  <si>
+    <t>[m] outer diameter of production casing</t>
+  </si>
+  <si>
+    <t>[m] outer diameter of tubing</t>
+  </si>
+  <si>
+    <t>[m] depth to top of cement</t>
   </si>
 </sst>
 </file>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52ECD9D-96F6-4DA0-914B-F81C4D5742D5}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D11" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,10 +581,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -602,10 +602,10 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -622,13 +622,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G2">
         <v>10</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -654,7 +654,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -709,7 +709,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -718,13 +718,13 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G5">
         <v>457.2</v>
@@ -738,7 +738,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -747,13 +747,13 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G6">
         <v>3.9</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -796,7 +796,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -805,10 +805,10 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>60</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -870,10 +870,10 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F10">
         <f>60 * 17.87</f>
@@ -897,7 +897,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -906,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8004289-A966-4581-8188-6DAA3855ADE3}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,10 +959,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -980,10 +980,10 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -1000,13 +1000,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G2">
         <v>10</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -1032,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1064,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1096,13 +1096,13 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G5">
         <v>457.2</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -1125,13 +1125,13 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G6">
         <v>3.9</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1154,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1174,7 +1174,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -1183,10 +1183,10 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>60</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -1212,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -1248,10 +1248,10 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F10">
         <f>60 * 17.87</f>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -1284,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1314,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38878A27-4F03-488B-A8C6-4048A6415AE1}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,10 +1337,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -1358,10 +1358,10 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -1378,13 +1378,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G2">
         <v>10</v>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -1410,7 +1410,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1442,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1474,13 +1474,13 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G5">
         <v>457.2</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -1503,13 +1503,13 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G6">
         <v>3.9</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1532,7 +1532,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -1561,10 +1561,10 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>60</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -1590,7 +1590,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -1626,10 +1626,10 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F10">
         <f>60 * 17.87</f>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -1662,7 +1662,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1693,7 +1693,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,10 +1711,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -1723,21 +1723,21 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>53</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -1754,7 +1754,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -1762,7 +1762,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -1771,7 +1771,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -1779,7 +1779,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -1788,15 +1788,15 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -1837,10 +1837,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -1849,12 +1849,12 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -1863,15 +1863,15 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -1880,10 +1880,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>